<commit_message>
update mock selectivities table to contain 5 tables
</commit_message>
<xml_diff>
--- a/mock-selectivities.xlsx
+++ b/mock-selectivities.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsiri\OneDrive\Desktop\TRI 1 2024\ENGR489\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793F1227-33B7-43E9-BA57-0ED7AF910D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F766B46-A976-47BC-9F6A-80F6AA2E72FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{201CF522-3B34-4405-87D9-E9A5A20A94A6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
   <si>
     <t>title</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>movie_info_idx</t>
+  </si>
+  <si>
+    <t>movie_link</t>
+  </si>
+  <si>
+    <t>complete_cast</t>
   </si>
 </sst>
 </file>
@@ -419,13 +425,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4605157F-DFA8-44D9-80C8-CE4C7208BA5D}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -463,19 +473,138 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>1000</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+      <c r="E3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>1000</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C5">
         <v>300</v>
       </c>
-      <c r="D3">
+      <c r="D5">
         <v>150</v>
       </c>
-      <c r="E3">
+      <c r="E5">
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>300</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+      <c r="E6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>300</v>
+      </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>150</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>150</v>
+      </c>
+      <c r="D9">
+        <v>100</v>
+      </c>
+      <c r="E9">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="E10">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>